<commit_message>
Set some prefilled fields to read_only
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_registration.xlsx
+++ b/xforms/xlsforms/death_registration.xlsx
@@ -1532,7 +1532,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1733,6 +1733,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="I8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added earliestDate to be configured from data managers in the form. This could be for example the earliest date that is valid for registering an outcome or a death or a migration.
it can be differentiated from round to round so that fieldworkers enter plausible dates.
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_registration.xlsx
+++ b/xforms/xlsforms/death_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-195" windowWidth="19200" windowHeight="7620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-195" windowWidth="19200" windowHeight="7620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>type</t>
   </si>
@@ -327,9 +327,6 @@
     <t>concat(${causeofdeathdiagnosed},${causofdeathnotdiagnosed})</t>
   </si>
   <si>
-    <t>. &lt; today()</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>processed</t>
   </si>
   <si>
-    <t>Date of death can not be in the future</t>
-  </si>
-  <si>
     <t>begin group</t>
   </si>
   <si>
@@ -376,12 +370,30 @@
   </si>
   <si>
     <t>concat(${individualId},'_DTH_',${fieldWorkerId})</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>earliestDate</t>
+  </si>
+  <si>
+    <t>Earliest date for death</t>
+  </si>
+  <si>
+    <t>. &lt; today() and &gt;${earliestDate}</t>
+  </si>
+  <si>
+    <t>Date of death can not be in the future or before the earliest date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -831,7 +843,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +904,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1580,13 +1601,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1604,10 +1625,12 @@
     <col min="11" max="11" width="19.125" style="5" customWidth="1"/>
     <col min="12" max="12" width="25.125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="5"/>
+    <col min="14" max="17" width="10.875" style="5"/>
+    <col min="18" max="18" width="10.875" style="24"/>
+    <col min="19" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1659,8 +1682,11 @@
       <c r="Q1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1710,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -1708,7 +1734,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1732,25 +1758,44 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="6" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="M5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="26">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>111</v>
-      </c>
       <c r="D6" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I6" s="22" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M6" s="22"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6" s="25"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1773,7 +1818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
@@ -1793,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
@@ -1813,16 +1858,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1832,16 +1877,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1851,18 +1896,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="23"/>
       <c r="I12" s="22"/>
       <c r="M12" s="22"/>
-    </row>
-    <row r="13" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -1878,16 +1924,16 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -1907,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>71</v>
       </c>
@@ -1918,7 +1964,7 @@
         <v>73</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1930,7 +1976,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>83</v>
       </c>
@@ -2007,7 +2053,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2044,16 +2090,16 @@
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -2861,7 +2907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2878,7 +2924,7 @@
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -2892,7 +2938,7 @@
         <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified condition on earliest date
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_registration.xlsx
+++ b/xforms/xlsforms/death_registration.xlsx
@@ -381,10 +381,10 @@
     <t>Earliest date for death</t>
   </si>
   <si>
-    <t>. &lt; today() and &gt;${earliestDate}</t>
-  </si>
-  <si>
     <t>Date of death can not be in the future or before the earliest date</t>
+  </si>
+  <si>
+    <t>. &lt; today() and . &gt;${earliestDate}</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -912,7 +912,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1607,7 +1607,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1924,10 +1924,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
workaround xlsform bug on converting default date
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_registration.xlsx
+++ b/xforms/xlsforms/death_registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
   <si>
     <t>type</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>. &lt; today() and . &gt;${earliestDate}</t>
+  </si>
+  <si>
+    <t>2014-06-01</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1604,10 +1607,10 @@
   <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1772,8 +1775,8 @@
       <c r="M5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="R5" s="26">
-        <v>41791</v>
+      <c r="R5" s="26" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
brought earliestDate default into settings
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/death_registration.xlsx
+++ b/xforms/xlsforms/death_registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>type</t>
   </si>
@@ -385,9 +385,6 @@
   </si>
   <si>
     <t>. &lt; today() and . &gt;${earliestDate}</t>
-  </si>
-  <si>
-    <t>2014-06-01</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1607,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1775,9 +1772,7 @@
       <c r="M5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="R5" s="26" t="s">
-        <v>123</v>
-      </c>
+      <c r="R5" s="26"/>
     </row>
     <row r="6" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">

</xml_diff>